<commit_message>
complete planning for sprint 2
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-1/report-sheet.xlsx
+++ b/sprint-backlog/sprint-1/report-sheet.xlsx
@@ -3,21 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8969F890-F1B8-4ECC-AF03-6F455E13F6DB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21BC0E4-EF46-494F-8E31-0A8A244518DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
     <sheet name="execution" sheetId="2" r:id="rId2"/>
     <sheet name="burndown" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">burndown!$A$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">burndown!$A$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">burndown!$B$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">burndown!$B$3:$G$3</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,9 +45,6 @@
     <t>J:3</t>
   </si>
   <si>
-    <t>1: 10-26-2018</t>
-  </si>
-  <si>
     <t>5: 10-22-2018</t>
   </si>
   <si>
@@ -118,6 +109,9 @@
   </si>
   <si>
     <t>acutal</t>
+  </si>
+  <si>
+    <t>1: 10-18-2018</t>
   </si>
 </sst>
 </file>
@@ -1668,17 +1662,17 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" activeCellId="4" sqref="D4 D5 D6 D7 D9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1687,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1699,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1733,13 +1727,13 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1756,7 +1750,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
@@ -1776,10 +1770,10 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1793,19 +1787,19 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1819,19 +1813,19 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1859,19 +1853,19 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1883,18 +1877,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF6B04-6D91-4CB2-B795-853A8560DA04}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" activeCellId="1" sqref="D9 D5:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1903,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1915,7 +1909,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1929,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1943,10 +1937,10 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1980,10 +1974,10 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1997,16 +1991,16 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2020,13 +2014,13 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2054,7 +2048,7 @@
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2066,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D36948-1878-4E62-8F83-9D21899FB0AC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
@@ -2074,7 +2068,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -2097,7 +2091,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>39</v>
@@ -2120,7 +2114,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>39</v>

</xml_diff>